<commit_message>
Development for SDM 35527
</commit_message>
<xml_diff>
--- a/Tickets/Normal Tickets/Ticket 35527 - SCT Transfer error/Test Plan.xlsx
+++ b/Tickets/Normal Tickets/Ticket 35527 - SCT Transfer error/Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_v2\WIP\Tickets\Normal Tickets\Ticket 35527 - SCT Transfer error\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC89F4A7-0AF0-42B4-AB21-3D0568E564FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D86D376-E8C7-4617-8C32-040EFC06AA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Test Case #</t>
   </si>
@@ -141,6 +141,30 @@
   </si>
   <si>
     <t>usp_Rest_Utility_Logon</t>
+  </si>
+  <si>
+    <t>Gnosis_Rest_Utility_Logon_For_Post</t>
+  </si>
+  <si>
+    <t>Set Up for Testing</t>
+  </si>
+  <si>
+    <t>Syspro.GnosisPORTOI</t>
+  </si>
+  <si>
+    <t>Syspro.GnosisPOST_PORTOI</t>
+  </si>
+  <si>
+    <t>usp_Post_Transfers_X_and_Donation</t>
+  </si>
+  <si>
+    <t>usp_Rest_Utility_Transfers_X_and_Donation_Post</t>
+  </si>
+  <si>
+    <t>usp_Rest_Utility_InventoryInternalSCTPost</t>
+  </si>
+  <si>
+    <t>usp_Post_InventoryInternalSCT</t>
   </si>
 </sst>
 </file>
@@ -254,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -298,57 +322,62 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,23 +399,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1800996</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>105061</xdr:rowOff>
+      <xdr:colOff>1724686</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>105038</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{421A7B38-74B8-4114-22ED-5C684C44D8B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C074587C-645B-C907-9BA7-13521663A3F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -402,8 +431,316 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="95250" y="4105275"/>
-          <a:ext cx="5525271" cy="2048161"/>
+          <a:off x="809625" y="4105275"/>
+          <a:ext cx="4734586" cy="1886213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>296929</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>565</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2805EC3-A6E5-BD9B-5EA9-A074CDDED750}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="6696075"/>
+          <a:ext cx="11850754" cy="4048690"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>478777</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>153303</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B945B78-BC26-568A-3E02-485AE0018D29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="828675" y="11229975"/>
+          <a:ext cx="18109552" cy="6468378"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>212043</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>152760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA139B9F-DFF5-E38D-D6F6-96C3430333F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="18192750"/>
+          <a:ext cx="17861868" cy="2581635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1172956</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>144048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B227A44-3720-774B-5896-059A7D7C9304}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="21431250"/>
+          <a:ext cx="9897856" cy="8402223"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>211787</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>38896</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A47F90C-BC98-21B2-25DF-9402862D16B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="30013275"/>
+          <a:ext cx="16032812" cy="5706271"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>221229</xdr:colOff>
+      <xdr:row>245</xdr:row>
+      <xdr:rowOff>678</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80956BFF-13C2-9A23-5DC6-94F31701D08E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="36652200"/>
+          <a:ext cx="15432654" cy="4858428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>248</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1658001</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>143211</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4614BD3B-35F8-FAE6-97CD-F6B50D41D431}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="41995725"/>
+          <a:ext cx="4667901" cy="2410161"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -784,11 +1121,11 @@
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -800,49 +1137,49 @@
       <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -854,49 +1191,56 @@
       <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>1</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>2</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>3</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
@@ -906,13 +1250,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -924,11 +1261,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <pane ySplit="5" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E252" sqref="E252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -943,58 +1280,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="22">
+      <c r="B2" s="28"/>
+      <c r="C2" s="18">
         <v>1</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="22" t="str">
+      <c r="B3" s="28"/>
+      <c r="C3" s="18" t="str">
         <f>'Test Cases'!B2</f>
         <v>Unit Testing</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="22" t="str">
+      <c r="B4" s="28"/>
+      <c r="C4" s="18" t="str">
         <f>'Test Cases'!D2</f>
         <v>1) SSMS</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="14" t="s">
         <v>19</v>
       </c>
@@ -1006,18 +1343,18 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="13" t="s">
         <v>31</v>
       </c>
@@ -1030,50 +1367,94 @@
       </c>
     </row>
     <row r="8" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C100" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C119" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C120" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D120" s="33"/>
+    </row>
+    <row r="212" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C212" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="213" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C213" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="247" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C247" s="15" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A8:F8"/>
@@ -1085,9 +1466,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1098,6 +1476,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a638d2c-e7c0-419c-9191-e92086f67d97">
@@ -1106,19 +1497,6 @@
     <TaxCatchAll xmlns="84e25877-5f26-4dc3-9598-48e40fb4ec5c" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1353,12 +1731,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1336CC8-439A-433F-AFCD-D3738BD4CF84}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{433CEB9C-4DCB-4DF9-8E44-99AD43459D1C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1a638d2c-e7c0-419c-9191-e92086f67d97"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="84e25877-5f26-4dc3-9598-48e40fb4ec5c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1372,9 +1747,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{433CEB9C-4DCB-4DF9-8E44-99AD43459D1C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1336CC8-439A-433F-AFCD-D3738BD4CF84}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1a638d2c-e7c0-419c-9191-e92086f67d97"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="84e25877-5f26-4dc3-9598-48e40fb4ec5c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>